<commit_message>
Rearranged files; about to add userType back into docWidgets, so both docWidgets and frames will have userType.  Endowing frames with userTypes allows a frame to exist without an assigned docWidget; endowing docWidgets with userTypes allows a docWidget to exist without being assigned to a frame.  The userTypes are matched when the document is selected
</commit_message>
<xml_diff>
--- a/doc/emdi_tables.xlsx
+++ b/doc/emdi_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\emdi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE78AFDC-1DFF-4FA2-A6EA-F89FF6D9E9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702E6D82-A1A3-4F55-9F37-D02B3C22062E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33395" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{6E634FF1-4F5E-45A3-A4E7-4B18B9E17CD3}"/>
+    <workbookView xWindow="41415" yWindow="6360" windowWidth="23040" windowHeight="12660" xr2:uid="{6E634FF1-4F5E-45A3-A4E7-4B18B9E17CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,15 +235,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>432262</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>99753</xdr:rowOff>
+      <xdr:colOff>417022</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>86418</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>955964</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>108067</xdr:rowOff>
+      <xdr:colOff>870239</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>96637</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -258,8 +258,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4056611" y="1629295"/>
-          <a:ext cx="1379913" cy="8314"/>
+          <a:off x="3846022" y="1353243"/>
+          <a:ext cx="1234267" cy="10219"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -585,32 +585,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E826A864-6B40-4CD2-82FA-B3579A3D0BF6}">
-  <dimension ref="D3:H15"/>
+  <dimension ref="D2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="3" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -631,33 +636,29 @@
       <c r="F7" t="s">
         <v>1</v>
       </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Enabled Dock frames to clear out when no content available from selected doc
</commit_message>
<xml_diff>
--- a/doc/emdi_tables.xlsx
+++ b/doc/emdi_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\emdi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702E6D82-A1A3-4F55-9F37-D02B3C22062E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708DE19E-11CB-4E9A-A9A2-5F45059E1A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41415" yWindow="6360" windowWidth="23040" windowHeight="12660" xr2:uid="{6E634FF1-4F5E-45A3-A4E7-4B18B9E17CD3}"/>
+    <workbookView xWindow="6435" yWindow="4830" windowWidth="16650" windowHeight="8280" xr2:uid="{6E634FF1-4F5E-45A3-A4E7-4B18B9E17CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>docs</t>
   </si>
@@ -236,13 +236,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>417022</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>86418</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>870239</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>96637</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -588,7 +588,7 @@
   <dimension ref="D2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,29 +636,33 @@
       <c r="F7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>10</v>

</xml_diff>